<commit_message>
feat: added data from x ray
</commit_message>
<xml_diff>
--- a/raio-x/raio-x-dados-dia-1.xlsx
+++ b/raio-x/raio-x-dados-dia-1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="124">
   <si>
     <t xml:space="preserve">Medidas de absorção - Diferentes materiais</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">aluminio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0</t>
   </si>
   <si>
     <t xml:space="preserve">0.11</t>
@@ -236,7 +239,7 @@
     <t xml:space="preserve">164.8</t>
   </si>
   <si>
-    <t xml:space="preserve">1.76</t>
+    <t xml:space="preserve">1.97</t>
   </si>
   <si>
     <t xml:space="preserve">86.4</t>
@@ -296,37 +299,31 @@
     <t xml:space="preserve">0.07</t>
   </si>
   <si>
-    <t xml:space="preserve">35.1</t>
+    <t xml:space="preserve">50.2</t>
   </si>
   <si>
-    <t xml:space="preserve">31.6</t>
+    <t xml:space="preserve">50.6</t>
   </si>
   <si>
-    <t xml:space="preserve">34.6</t>
+    <t xml:space="preserve">48.1</t>
   </si>
   <si>
-    <t xml:space="preserve">32.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33.5</t>
+    <t xml:space="preserve">52.2</t>
   </si>
   <si>
     <t xml:space="preserve">0.12</t>
   </si>
   <si>
-    <t xml:space="preserve">4.20</t>
+    <t xml:space="preserve">6.1</t>
   </si>
   <si>
-    <t xml:space="preserve">4.95</t>
+    <t xml:space="preserve">5.9</t>
   </si>
   <si>
-    <t xml:space="preserve">3.72</t>
+    <t xml:space="preserve">7.0</t>
   </si>
   <si>
-    <t xml:space="preserve">4.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.58</t>
+    <t xml:space="preserve">7.1</t>
   </si>
   <si>
     <t xml:space="preserve">0.18</t>
@@ -730,8 +727,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1017,32 +1014,27 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>36</v>
+      <c r="C8" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>37</v>
+      <c r="D8" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>38</v>
+      <c r="E8" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>39</v>
+      <c r="F8" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>40</v>
+      <c r="G8" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
@@ -1062,22 +1054,22 @@
         <v>34</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1103,22 +1095,22 @@
         <v>34</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1144,22 +1136,22 @@
         <v>34</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -1185,22 +1177,22 @@
         <v>34</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1226,22 +1218,22 @@
         <v>34</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -1267,22 +1259,22 @@
         <v>34</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1308,28 +1300,28 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
@@ -1346,31 +1338,31 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
@@ -1386,32 +1378,27 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
-        <v>83</v>
+      <c r="A17" s="1" t="s">
+        <v>84</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>90</v>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>91</v>
+      <c r="C17" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>92</v>
+      <c r="D17" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>93</v>
+      <c r="E17" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>94</v>
+      <c r="F17" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>95</v>
+      <c r="G17" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
@@ -1428,31 +1415,31 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3" t="s">
-        <v>97</v>
+      <c r="C18" s="3" t="s">
+        <v>86</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>98</v>
+      <c r="D18" s="3" t="s">
+        <v>87</v>
       </c>
-      <c r="J18" s="3" t="s">
-        <v>99</v>
+      <c r="E18" s="3" t="s">
+        <v>88</v>
       </c>
-      <c r="K18" s="8" t="s">
-        <v>100</v>
+      <c r="F18" s="3" t="s">
+        <v>89</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>101</v>
+      <c r="G18" s="3" t="s">
+        <v>90</v>
       </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -1469,31 +1456,31 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
-        <v>103</v>
+      <c r="C19" s="2" t="s">
+        <v>92</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>104</v>
+      <c r="D19" s="2" t="s">
+        <v>93</v>
       </c>
-      <c r="J19" s="3" t="s">
-        <v>105</v>
+      <c r="E19" s="2" t="s">
+        <v>94</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>106</v>
+      <c r="F19" s="2" t="s">
+        <v>92</v>
       </c>
-      <c r="L19" s="3" t="s">
-        <v>107</v>
+      <c r="G19" s="2" t="s">
+        <v>95</v>
       </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -1510,31 +1497,31 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
-        <v>109</v>
+      <c r="C20" s="2" t="s">
+        <v>97</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>110</v>
+      <c r="D20" s="2" t="s">
+        <v>98</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>109</v>
+      <c r="E20" s="2" t="s">
+        <v>99</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>33</v>
+      <c r="F20" s="2" t="s">
+        <v>100</v>
       </c>
-      <c r="L20" s="3" t="s">
-        <v>111</v>
+      <c r="G20" s="2" t="s">
+        <v>98</v>
       </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="3"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
@@ -1551,31 +1538,31 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>113</v>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>102</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>114</v>
+      <c r="I21" s="3" t="s">
+        <v>103</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>113</v>
+      <c r="J21" s="3" t="s">
+        <v>104</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>115</v>
+      <c r="K21" s="3" t="s">
+        <v>105</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>116</v>
+      <c r="L21" s="3" t="s">
+        <v>106</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -1592,31 +1579,31 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>117</v>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3" t="s">
+        <v>108</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>118</v>
+      <c r="I22" s="3" t="s">
+        <v>109</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>119</v>
+      <c r="J22" s="3" t="s">
+        <v>108</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>120</v>
+      <c r="K22" s="3" t="s">
+        <v>33</v>
       </c>
-      <c r="G22" s="10" t="s">
-        <v>121</v>
+      <c r="L22" s="3" t="s">
+        <v>110</v>
       </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -1632,32 +1619,32 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>112</v>
+      <c r="A23" s="1" t="s">
+        <v>111</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>28</v>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>122</v>
+      <c r="C23" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>123</v>
+      <c r="D23" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>124</v>
+      <c r="E23" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>123</v>
+      <c r="F23" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="G23" s="10" t="s">
-        <v>124</v>
+      <c r="G23" s="7" t="s">
+        <v>22</v>
       </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -1672,12 +1659,33 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -1694,18 +1702,32 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
+      <c r="A25" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -1722,13 +1744,27 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="A26" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>123</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1750,13 +1786,8 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1778,8 +1809,6 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>

</xml_diff>